<commit_message>
ajout des résultats d'experimentation
</commit_message>
<xml_diff>
--- a/experimentation.xlsx
+++ b/experimentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/Ecole/Informatique/PyomoSolvers_macOS/circle_optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE39382F-D75C-5440-B077-E4DB5C4C3E57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8DEFAB-1437-694E-A27D-33D7DCB5011D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="460" windowWidth="21160" windowHeight="16680" xr2:uid="{A59636CF-62F1-3643-8B80-4090D43F6B23}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="21160" windowHeight="16680" xr2:uid="{A59636CF-62F1-3643-8B80-4090D43F6B23}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="19">
   <si>
     <t>MBH</t>
   </si>
@@ -71,24 +71,33 @@
   <si>
     <t>Cplx</t>
   </si>
+  <si>
+    <t>476.208812</t>
+  </si>
+  <si>
+    <t>480.076336</t>
+  </si>
+  <si>
+    <t>379.938626</t>
+  </si>
+  <si>
+    <t>355.260012</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="173" formatCode="0.0000000000000000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFF2F2F2"/>
-      <name val="Monaco"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -100,6 +109,18 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -123,11 +144,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="173" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,6 +167,1250 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1600" b="1"/>
+              <a:t>Influence</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" sz="1600" b="1" baseline="0"/>
+              <a:t> de la perturbation sur l'efficacité de l'algorithme</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR" sz="1600" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21530484036412173"/>
+          <c:y val="5.3900709219858157E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10506026849900643"/>
+          <c:y val="0.17046808510638298"/>
+          <c:w val="0.83191639234503156"/>
+          <c:h val="0.75860992907801406"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Feuil1!$C$15:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.01</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.03</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.0000000000000007E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.09</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.5000000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.4999999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$F$15:$F$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>7.612544220694518E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1240175211205575E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.5864802333581856E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5599658248978384E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5421069729224602E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.2758289109908658E-6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.6392051899628505E-6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.7703716104421852E-8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.765934228351911E-6</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.7584344105419046E-6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.1549098884234911E-7</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.5377509049903446E-6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2038305096296774E-6</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2016704451280329E-5</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.1594166116446409E-6</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.9303860390721823E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.6291252292459838E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.3699366602032095E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.5034245752350886E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E550-6B45-91BB-7233C71BA77E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$I$15:$I$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.4200000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000010-E550-6B45-91BB-7233C71BA77E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="246683200"/>
+        <c:axId val="250163792"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="246683200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1400"/>
+                  <a:t>Taille</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1400" baseline="0"/>
+                  <a:t> de la pertubation</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.39299162764647061"/>
+              <c:y val="0.94326241134751776"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="250163792"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="250163792"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1800"/>
+                  <a:t>∆</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" sz="1800" baseline="-25000"/>
+                  <a:t>relatif</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.95181417087626974"/>
+              <c:y val="0.50108516222706201"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="246683200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>769418</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DF277000-1653-0C4F-8AC3-D1717C210947}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,21 +1710,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E38A7BC-2DEB-FE4D-B23E-CC8068DBDAD8}">
-  <dimension ref="A6:H14"/>
+  <dimension ref="A6:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
     <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -479,7 +1748,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -489,7 +1758,7 @@
       <c r="C7">
         <v>0.3</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <v>7.5781562667006294E-2</v>
       </c>
       <c r="E7" s="3">
@@ -506,17 +1775,14 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>192.03359799999899</v>
       </c>
-      <c r="C8">
-        <v>0.3</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="D8" s="4">
         <v>7.4648145970688695E-2</v>
       </c>
       <c r="E8" s="3">
@@ -533,17 +1799,17 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>247.53299999999999</v>
       </c>
       <c r="C9">
         <v>0.3</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <v>7.5781949661743606E-2</v>
       </c>
       <c r="E9" s="3">
@@ -560,7 +1826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -570,7 +1836,7 @@
       <c r="C10">
         <v>0.3</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="4">
         <v>7.5518477897416794E-2</v>
       </c>
       <c r="E10" s="3">
@@ -587,12 +1853,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
-      <c r="C11">
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="2">
         <v>0.3</v>
+      </c>
+      <c r="D11" s="4">
+        <v>7.5781670824573696E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ref="F11:F14" si="0">($E$7-D11)/$E$7</f>
+        <v>4.1592117147189784E-6</v>
       </c>
       <c r="G11" t="s">
         <v>7</v>
@@ -601,12 +1880,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="C12">
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="2">
         <v>0.1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>7.5781750762208694E-2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>3.1043748174833444E-6</v>
       </c>
       <c r="G12" t="s">
         <v>7</v>
@@ -615,12 +1907,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
-      <c r="C13">
+      <c r="B13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2">
         <v>0.5</v>
+      </c>
+      <c r="D13" s="4">
+        <v>7.5781854408789595E-2</v>
+      </c>
+      <c r="E13" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>1.7366806417626102E-6</v>
       </c>
       <c r="G13" t="s">
         <v>7</v>
@@ -629,21 +1934,580 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C14">
+      <c r="B14" s="6"/>
+      <c r="C14" s="5">
         <v>0.3</v>
       </c>
-      <c r="G14" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="5" t="s">
         <v>11</v>
       </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1E-3</v>
+      </c>
+      <c r="D15" s="1">
+        <v>7.5205092298204407E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F15">
+        <f>($E$7-D15)/$E$7</f>
+        <v>7.612544220694518E-3</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I15">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="6">
+        <v>0.01</v>
+      </c>
+      <c r="D16" s="1">
+        <v>7.4930183217203405E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F16">
+        <f>($E$7-D16)/$E$7</f>
+        <v>1.1240175211205575E-2</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I16">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="D17" s="1">
+        <v>7.5358631450964095E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F17">
+        <f>($E$7-D17)/$E$7</f>
+        <v>5.5864802333581856E-3</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="D18" s="1">
+        <v>7.5512204737531105E-2</v>
+      </c>
+      <c r="E18" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F18">
+        <f>($E$7-D18)/$E$7</f>
+        <v>3.5599658248978384E-3</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="6">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>7.5513558116801799E-2</v>
+      </c>
+      <c r="E19" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F19">
+        <f>($E$7-D19)/$E$7</f>
+        <v>3.5421069729224602E-3</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I19">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.09</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7.5781434641132905E-2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F20">
+        <f>($E$7-D20)/$E$7</f>
+        <v>7.2758289109908658E-6</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I20">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7.5781786013686903E-2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F21">
+        <f>($E$7-D21)/$E$7</f>
+        <v>2.6392051899628505E-6</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D22" s="1">
+        <v>7.57819816449955E-2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F22">
+        <f>($E$7-D22)/$E$7</f>
+        <v>5.7703716104421852E-8</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <v>331.66284999999999</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="1">
+        <v>7.5781852191894705E-2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F23">
+        <f>($E$7-D23)/$E$7</f>
+        <v>1.765934228351911E-6</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I23">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="6">
+        <v>0.25</v>
+      </c>
+      <c r="D24" s="1">
+        <v>7.5781852760245794E-2</v>
+      </c>
+      <c r="E24" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ref="F24:F26" si="1">($E$7-D24)/$E$7</f>
+        <v>1.7584344105419046E-6</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1">
+        <v>247.53299999999999</v>
+      </c>
+      <c r="C25">
+        <v>0.3</v>
+      </c>
+      <c r="D25" s="4">
+        <v>7.5781977265761205E-2</v>
+      </c>
+      <c r="E25" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>1.1549098884234911E-7</v>
+      </c>
+      <c r="G25" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" t="s">
+        <v>11</v>
+      </c>
+      <c r="I25">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" s="6">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D26" s="1">
+        <v>7.5781339010178E-2</v>
+      </c>
+      <c r="E26" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>8.5377509049903446E-6</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I26">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="1">
+        <v>367.65131200000002</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7.5781667443272804E-2</v>
+      </c>
+      <c r="E27" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F27">
+        <f>($E$7-D27)/$E$7</f>
+        <v>4.2038305096296774E-6</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I27">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C28" s="6">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>7.5781075368168999E-2</v>
+      </c>
+      <c r="E28" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F28">
+        <f>($E$7-D28)/$E$7</f>
+        <v>1.2016704451280329E-5</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I28">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="1">
+        <v>439.34189900000001</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D29" s="4">
+        <v>7.57816708090462E-2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F29">
+        <f>($E$7-D29)/$E$7</f>
+        <v>4.1594166116446409E-6</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I29">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1">
+        <v>317.68772799999999</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D30" s="4">
+        <v>7.5408351572021901E-2</v>
+      </c>
+      <c r="E30" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F30">
+        <f>($E$7-D30)/$E$7</f>
+        <v>4.9303860390721823E-3</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I30">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="1">
+        <v>344.51567</v>
+      </c>
+      <c r="C31" s="6">
+        <v>0.7</v>
+      </c>
+      <c r="D31" s="4">
+        <v>7.5052271784410401E-2</v>
+      </c>
+      <c r="E31" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F31">
+        <f>($E$7-D31)/$E$7</f>
+        <v>9.6291252292459838E-3</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="1">
+        <v>541.79477199999997</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="D32" s="4">
+        <v>7.5147695594943498E-2</v>
+      </c>
+      <c r="E32" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F32">
+        <f>($E$7-D32)/$E$7</f>
+        <v>8.3699366602032095E-3</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I32">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="1">
+        <v>466.34943600000003</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="D33" s="4">
+        <v>7.5061797629615096E-2</v>
+      </c>
+      <c r="E33" s="3">
+        <v>7.5781986017897707E-2</v>
+      </c>
+      <c r="F33">
+        <f>($E$7-D33)/$E$7</f>
+        <v>9.5034245752350886E-3</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I33">
+        <v>1.4200000000000001E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="E34" s="3"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout de commentaire dans le code
</commit_message>
<xml_diff>
--- a/experimentation.xlsx
+++ b/experimentation.xlsx
@@ -8,13 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/Ecole/Informatique/PyomoSolvers_macOS/circle_optimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD8DEFAB-1437-694E-A27D-33D7DCB5011D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37ACB770-54EA-9C4B-8EE9-37E3FEE174EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21160" windowHeight="16680" xr2:uid="{A59636CF-62F1-3643-8B80-4090D43F6B23}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Feuil1!$C$15:$C$33</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Feuil1!$F$15:$F$33</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Feuil1!$F$15:$F$33</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Feuil1!$I$15:$I$33</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Feuil1!$I$15:$I$33</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Feuil1!$C$15:$C$33</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Feuil1!$F$15:$F$33</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Feuil1!$I$15:$I$33</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Feuil1!$C$15:$C$33</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Feuil1!$F$15:$F$33</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Feuil1!$I$15:$I$33</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Feuil1!$C$15:$C$33</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -272,15 +286,26 @@
           <c:order val="0"/>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -517,6 +542,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="246683200"/>
         <c:axId val="250163792"/>
@@ -1712,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E38A7BC-2DEB-FE4D-B23E-CC8068DBDAD8}">
   <dimension ref="A6:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>